<commit_message>
more tests use getVocabulary instead check authorization before everything bug fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/importapi/excel/simple_import_term_missing_lang.xlsx
+++ b/src/test/resources/importapi/excel/simple_import_term_missing_lang.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">prefLabel_fi</t>
   </si>
   <si>
     <t xml:space="preserve">prefLabel_sv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">altLabel_fi</t>
   </si>
   <si>
     <t xml:space="preserve">altLabel</t>
@@ -186,10 +189,10 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.5"/>
@@ -211,60 +214,60 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>